<commit_message>
fixed quite a few minor stuff. THE EDIT on DIARY IS NOT WORKING !!
</commit_message>
<xml_diff>
--- a/Files/0000-1000/5/B5_RequestList.xlsx
+++ b/Files/0000-1000/5/B5_RequestList.xlsx
@@ -25,7 +25,7 @@
     <t>ОФИС гр. РУСЕ и ОФИС гр. СОФИЯ</t>
   </si>
   <si>
-    <t>ЗАЯВКА № B5 / Дата 21.07.2016</t>
+    <t>ЗАЯВКА № B5 / Дата 28.07.2016</t>
   </si>
   <si>
     <t>7.2 ФИЗИКОХИМИЧНО И ОРГАНОЛЕПТИЧНО ИЗПИТВАНЕ</t>
@@ -64,7 +64,7 @@
     <t>asd</t>
   </si>
   <si>
-    <t>Срок за изпитване: 5 дни</t>
+    <t>Срок за изпитване: 4 дни</t>
   </si>
   <si>
     <t>Приел пробата......</t>

</xml_diff>

<commit_message>
Edit bug and Tests changing (methods) bug were fixed.
Redirecting, opening, redirecting and scrolling to the selected protocol from Requests was corrected
And a bug in the archived protocols results display was also fixed
</commit_message>
<xml_diff>
--- a/Files/0000-1000/5/B5_RequestList.xlsx
+++ b/Files/0000-1000/5/B5_RequestList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">ФК 404-4   </t>
   </si>
@@ -25,7 +25,7 @@
     <t>ОФИС гр. РУСЕ и ОФИС гр. СОФИЯ</t>
   </si>
   <si>
-    <t>ЗАЯВКА № B5 / Дата 28.07.2016</t>
+    <t>ЗАЯВКА № B5 / Дата 30.07.2016</t>
   </si>
   <si>
     <t>7.2 ФИЗИКОХИМИЧНО И ОРГАНОЛЕПТИЧНО ИЗПИТВАНЕ</t>
@@ -55,6 +55,18 @@
     <t>1. asd</t>
   </si>
   <si>
+    <t>TTTTTTTTTT1</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>asd2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remark ... </t>
+  </si>
+  <si>
     <t>TestMethod</t>
   </si>
   <si>
@@ -64,7 +76,10 @@
     <t>asd</t>
   </si>
   <si>
-    <t>Срок за изпитване: 4 дни</t>
+    <t>2. product</t>
+  </si>
+  <si>
+    <t>Срок за изпитване: 2 дни</t>
   </si>
   <si>
     <t>Приел пробата......</t>
@@ -483,29 +498,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75">
+    <row r="1" ht="17.4">
       <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="3" ht="18.75">
+    <row r="3" ht="17.4">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -516,7 +531,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" ht="18.75">
+    <row r="4" ht="17.4">
       <c r="A4" s="1"/>
       <c r="B4" s="8" t="s">
         <v>2</v>
@@ -532,7 +547,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="7" ht="18.75">
+    <row r="7" ht="17.4">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
@@ -597,27 +612,59 @@
         <v>15</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>17</v>
+      <c r="D13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -625,8 +672,8 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>